<commit_message>
Added my name in myteams.txt
</commit_message>
<xml_diff>
--- a/segue_training/Python Batch 1- Foundation Training Plan - March 2025.xlsx
+++ b/segue_training/Python Batch 1- Foundation Training Plan - March 2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{51B6E137-384B-4C07-9D44-EBBDEECF854F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{210C6419-6026-4278-8B84-B76947072160}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="2" xr2:uid="{7099B43E-2618-4751-BD83-56A694EF2D35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{7099B43E-2618-4751-BD83-56A694EF2D35}"/>
   </bookViews>
   <sheets>
     <sheet name="Workshop Schedule" sheetId="9" r:id="rId1"/>
@@ -1001,12 +1001,48 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1015,42 +1051,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273E7271-0C0D-499A-952D-65714BF1C1E7}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="107" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA07742-60C7-481A-82E3-F03F5DD0CE9E}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1955,13 +1955,13 @@
       </c>
     </row>
     <row r="2" spans="1:11" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="63">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="51" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="18" t="s">
@@ -1980,9 +1980,9 @@
       <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:11" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2002,9 +2002,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" customFormat="1" ht="81" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
@@ -2024,9 +2024,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="18" t="s">
         <v>19</v>
       </c>
@@ -2043,9 +2043,9 @@
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:11" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="64"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="18" t="s">
         <v>21</v>
       </c>
@@ -2065,13 +2065,13 @@
       </c>
     </row>
     <row r="7" spans="1:11" customFormat="1" ht="81" x14ac:dyDescent="0.3">
-      <c r="A7" s="67">
+      <c r="A7" s="54">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="55" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -2093,9 +2093,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="60"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="14" t="s">
         <v>26</v>
       </c>
@@ -2112,13 +2112,13 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:11" s="17" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="63">
+      <c r="A9" s="51">
         <v>3</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="51" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -2137,9 +2137,9 @@
       <c r="I9" s="39"/>
     </row>
     <row r="10" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="19" t="s">
         <v>32</v>
       </c>
@@ -2156,9 +2156,9 @@
       <c r="I10" s="39"/>
     </row>
     <row r="11" spans="1:11" s="17" customFormat="1" ht="81" x14ac:dyDescent="0.3">
-      <c r="A11" s="65"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="19" t="s">
         <v>34</v>
       </c>
@@ -2175,9 +2175,9 @@
       <c r="I11" s="39"/>
     </row>
     <row r="12" spans="1:11" s="17" customFormat="1" ht="81" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="19" t="s">
         <v>36</v>
       </c>
@@ -2194,9 +2194,9 @@
       <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:11" s="17" customFormat="1" ht="178.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="64"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
       <c r="D13" s="19" t="s">
         <v>38</v>
       </c>
@@ -2213,9 +2213,9 @@
       <c r="I13" s="39"/>
     </row>
     <row r="14" spans="1:11" s="17" customFormat="1" ht="178.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="51" t="s">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="57" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="18" t="s">
@@ -2234,9 +2234,9 @@
       <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:11" s="17" customFormat="1" ht="113.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="56"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="18" t="s">
         <v>42</v>
       </c>
@@ -2253,9 +2253,9 @@
       <c r="I15" s="40"/>
     </row>
     <row r="16" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="52"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="59"/>
       <c r="D16" s="32" t="s">
         <v>44</v>
       </c>
@@ -2270,12 +2270,12 @@
       <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:11" s="17" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="63" t="s">
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E17" s="23" t="s">
@@ -2291,10 +2291,10 @@
       <c r="I17" s="39"/>
     </row>
     <row r="18" spans="1:11" s="17" customFormat="1" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="64"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="23" t="s">
         <v>47</v>
       </c>
@@ -2308,9 +2308,9 @@
       <c r="I18" s="39"/>
     </row>
     <row r="19" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="64"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="18" t="s">
         <v>44</v>
       </c>
@@ -2325,12 +2325,12 @@
       <c r="I19" s="40"/>
     </row>
     <row r="20" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="63" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="57" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="18" t="s">
@@ -2344,10 +2344,10 @@
       <c r="I20" s="40"/>
     </row>
     <row r="21" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="52"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="18" t="s">
         <v>50</v>
       </c>
@@ -2361,7 +2361,7 @@
     <row r="22" spans="1:11" s="17" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="55" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -2378,13 +2378,13 @@
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:11" ht="145.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A23" s="59">
+      <c r="A23" s="55">
         <v>4</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="60"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="14" t="s">
         <v>96</v>
       </c>
@@ -2404,9 +2404,9 @@
       <c r="K23" s="17"/>
     </row>
     <row r="24" spans="1:11" ht="226.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="66"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="59" t="s">
+      <c r="A24" s="60"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="55" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="14" t="s">
@@ -2428,9 +2428,9 @@
       <c r="K24" s="17"/>
     </row>
     <row r="25" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="60"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="31" t="s">
         <v>44</v>
       </c>
@@ -2445,9 +2445,9 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:11" ht="162" x14ac:dyDescent="0.3">
-      <c r="A26" s="66"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="59" t="s">
+      <c r="A26" s="60"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="55" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="11" t="s">
@@ -2469,9 +2469,9 @@
       <c r="K26" s="17"/>
     </row>
     <row r="27" spans="1:11" ht="48.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="11" t="s">
         <v>56</v>
       </c>
@@ -2487,9 +2487,9 @@
       <c r="K27" s="17"/>
     </row>
     <row r="28" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="66"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="60"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="56"/>
       <c r="D28" s="31" t="s">
         <v>44</v>
       </c>
@@ -2504,9 +2504,9 @@
       <c r="I28" s="14"/>
     </row>
     <row r="29" spans="1:11" s="17" customFormat="1" ht="81" x14ac:dyDescent="0.3">
-      <c r="A29" s="66"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="59" t="s">
+      <c r="A29" s="60"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="55" t="s">
         <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
@@ -2523,9 +2523,9 @@
       <c r="I29" s="41"/>
     </row>
     <row r="30" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="66"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="14" t="s">
         <v>103</v>
       </c>
@@ -2540,9 +2540,9 @@
       <c r="I30" s="41"/>
     </row>
     <row r="31" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="66"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="60"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="31" t="s">
         <v>44</v>
       </c>
@@ -2557,9 +2557,9 @@
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:11" s="17" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="59" t="s">
+      <c r="A32" s="60"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="55" t="s">
         <v>58</v>
       </c>
       <c r="D32" s="14" t="s">
@@ -2576,9 +2576,9 @@
       <c r="I32" s="41"/>
     </row>
     <row r="33" spans="1:11" s="17" customFormat="1" ht="113.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
+      <c r="A33" s="60"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="14" t="s">
         <v>4</v>
       </c>
@@ -2593,9 +2593,9 @@
       <c r="I33" s="14"/>
     </row>
     <row r="34" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="66"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="60"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="31" t="s">
         <v>44</v>
       </c>
@@ -2610,9 +2610,9 @@
       <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:11" s="17" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="66"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="59" t="s">
+      <c r="A35" s="60"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="55" t="s">
         <v>59</v>
       </c>
       <c r="D35" s="14" t="s">
@@ -2631,9 +2631,9 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:11" s="17" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="31" t="s">
         <v>60</v>
       </c>
@@ -2648,9 +2648,9 @@
       <c r="I36" s="41"/>
     </row>
     <row r="37" spans="1:11" s="17" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="66"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="60"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="31" t="s">
         <v>44</v>
       </c>
@@ -2665,9 +2665,9 @@
       <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:11" s="17" customFormat="1" ht="113.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="66"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="59" t="s">
+      <c r="A38" s="60"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="55" t="s">
         <v>61</v>
       </c>
       <c r="D38" s="14" t="s">
@@ -2684,9 +2684,9 @@
       <c r="I38" s="41"/>
     </row>
     <row r="39" spans="1:11" s="17" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="66"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="37" t="s">
         <v>113</v>
       </c>
@@ -2701,13 +2701,13 @@
       <c r="I39" s="41"/>
     </row>
     <row r="40" spans="1:11" s="17" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="51">
+      <c r="A40" s="57">
         <v>6</v>
       </c>
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="57" t="s">
         <v>62</v>
       </c>
       <c r="D40" s="40" t="s">
@@ -2724,9 +2724,9 @@
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:11" s="17" customFormat="1" ht="113.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="56"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="18" t="s">
         <v>64</v>
       </c>
@@ -2741,9 +2741,9 @@
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:11" s="17" customFormat="1" ht="113.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="56"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="51" t="s">
+      <c r="A42" s="58"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="57" t="s">
         <v>65</v>
       </c>
       <c r="D42" s="18" t="s">
@@ -2760,9 +2760,9 @@
       <c r="I42" s="18"/>
     </row>
     <row r="43" spans="1:11" s="17" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="52"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="52"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
       <c r="D43" s="18" t="s">
         <v>117</v>
       </c>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="44" spans="1:11" s="17" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="51" t="s">
+      <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="51" t="s">
+      <c r="D44" s="57" t="s">
         <v>118</v>
       </c>
       <c r="E44" s="35" t="s">
@@ -2799,9 +2799,9 @@
     </row>
     <row r="45" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="33" t="s">
         <v>69</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="K45" s="17"/>
     </row>
     <row r="46" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="57">
+      <c r="A46" s="61">
         <v>7</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="61" t="s">
+      <c r="C46" s="63" t="s">
         <v>71</v>
       </c>
       <c r="D46" s="25" t="s">
@@ -2839,9 +2839,9 @@
       <c r="I46" s="42"/>
     </row>
     <row r="47" spans="1:11" ht="69" x14ac:dyDescent="0.3">
-      <c r="A47" s="58"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="62"/>
+      <c r="A47" s="62"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="64"/>
       <c r="D47" s="25" t="s">
         <v>73</v>
       </c>
@@ -2858,13 +2858,13 @@
       <c r="I47" s="42"/>
     </row>
     <row r="48" spans="1:11" ht="69" x14ac:dyDescent="0.3">
-      <c r="A48" s="51">
+      <c r="A48" s="57">
         <v>8</v>
       </c>
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="54" t="s">
+      <c r="C48" s="66" t="s">
         <v>85</v>
       </c>
       <c r="D48" s="29" t="s">
@@ -2883,9 +2883,9 @@
       <c r="I48" s="43"/>
     </row>
     <row r="49" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="52"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="55"/>
+      <c r="A49" s="59"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="67"/>
       <c r="D49" s="29" t="s">
         <v>78</v>
       </c>
@@ -2909,20 +2909,12 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B21"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B46:B47"/>
@@ -2939,12 +2931,20 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A9:A21"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B9:B21"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2953,6 +2953,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2427474e-60f8-4f75-abfc-98841d67cf98" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004AC3E03F954406448D57A63F810EB967" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="52e6b73825859cad1527a80b81e763dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -3066,27 +3086,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2427474e-60f8-4f75-abfc-98841d67cf98" ContentTypeId="0x01" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6973C3B0-8CE8-4B28-810C-8D7411FE369B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DA35318-3F34-48CC-8A55-62D58D2CBB91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEF3DC22-7D19-493B-89C6-F7B61160F957}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0C58A0-E478-4B1A-8F74-6643D6C5F2A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3100,29 +3125,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEF3DC22-7D19-493B-89C6-F7B61160F957}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DA35318-3F34-48CC-8A55-62D58D2CBB91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6973C3B0-8CE8-4B28-810C-8D7411FE369B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>